<commit_message>
need to fix datagetter
</commit_message>
<xml_diff>
--- a/mydata.xlsx
+++ b/mydata.xlsx
@@ -1,130 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/98de4cb101dd5aa6/Dev/Excel project/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_FC91EDF68BBC5EDAFE92E0152ACE22D1CF754952" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{040D24C8-493B-41E0-9CE2-806EE2DA9FC4}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="19200" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Metadata" sheetId="2" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Metadata" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>United Kingdom Manufacturing PMI</t>
-  </si>
-  <si>
-    <t>units</t>
-  </si>
-  <si>
-    <t>points</t>
-  </si>
-  <si>
-    <t>original_source</t>
-  </si>
-  <si>
-    <t>S&amp;P Global</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>indicator</t>
-  </si>
-  <si>
-    <t>manufacturing pmi</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>united kingdom</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>Trading Economics</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>united-kingdom/manufacturing-pmi</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>Markit/CIPS UK Manufacturing Purchasing Managers’ Index measures the performance of the manufacturing sector and is derived from a survey of 600 industrial companies. The Manufacturing Purchasing Managers Index is based on five individual indexes with the following weights: New Orders (30 percent), Output (25 percent), Employment (20 percent), Suppliers’ Delivery Times (15 percent) and Stock of Items Purchased (10 percent), with the Delivery Times index inverted so that it moves in a comparable direction. A reading above 50 indicates an expansion of the manufacturing sector compared to the previous month; below 50 represents a contraction; while 50 indicates no change. This is only a limited sample of PMI headline data displayed on the Customer’s service, under licence from S&amp;P Global. Full historic PMI headline data and all other PMI sub-index data and histories are available on subscription from S&amp;P Global. Contact economics@spglobal.com for more details.</t>
-  </si>
-  <si>
-    <t>frequency</t>
-  </si>
-  <si>
-    <t>MS</t>
-  </si>
-  <si>
-    <t>start_date</t>
-  </si>
-  <si>
-    <t>2022-03-01</t>
-  </si>
-  <si>
-    <t>end_date</t>
-  </si>
-  <si>
-    <t>2025-03-01</t>
-  </si>
-  <si>
-    <t>min_value</t>
-  </si>
-  <si>
-    <t>max_value</t>
-  </si>
-  <si>
-    <t>length</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -139,46 +50,96 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -466,319 +427,324 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>United Kingdom Manufacturing PMI</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
         <v>44621</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>55.2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
+    <row r="3">
+      <c r="A3" s="2" t="n">
         <v>44652</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>55.8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+    <row r="4">
+      <c r="A4" s="2" t="n">
         <v>44682</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>54.6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+    <row r="5">
+      <c r="A5" s="2" t="n">
         <v>44713</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>52.8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+    <row r="6">
+      <c r="A6" s="2" t="n">
         <v>44743</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n">
         <v>52.1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+    <row r="7">
+      <c r="A7" s="2" t="n">
         <v>44774</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="n">
         <v>47.3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+    <row r="8">
+      <c r="A8" s="2" t="n">
         <v>44805</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="n">
         <v>48.4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
+    <row r="9">
+      <c r="A9" s="2" t="n">
         <v>44835</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="n">
         <v>46.2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
+    <row r="10">
+      <c r="A10" s="2" t="n">
         <v>44866</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="n">
         <v>46.5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
+    <row r="11">
+      <c r="A11" s="2" t="n">
         <v>44896</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="n">
         <v>45.3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
+    <row r="12">
+      <c r="A12" s="2" t="n">
         <v>44927</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="n">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
+    <row r="13">
+      <c r="A13" s="2" t="n">
         <v>44958</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="n">
         <v>49.3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
+    <row r="14">
+      <c r="A14" s="2" t="n">
         <v>44986</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="n">
         <v>47.9</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
+    <row r="15">
+      <c r="A15" s="2" t="n">
         <v>45017</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="n">
         <v>47.8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
+    <row r="16">
+      <c r="A16" s="2" t="n">
         <v>45047</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="n">
         <v>47.1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
+    <row r="17">
+      <c r="A17" s="2" t="n">
         <v>45078</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="n">
         <v>46.5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
+    <row r="18">
+      <c r="A18" s="2" t="n">
         <v>45108</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="n">
         <v>45.3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
+    <row r="19">
+      <c r="A19" s="2" t="n">
         <v>45139</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="n">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
+    <row r="20">
+      <c r="A20" s="2" t="n">
         <v>45170</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="n">
         <v>44.3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
+    <row r="21">
+      <c r="A21" s="2" t="n">
         <v>45200</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="n">
         <v>44.8</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
+    <row r="22">
+      <c r="A22" s="2" t="n">
         <v>45231</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="n">
         <v>47.2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="2">
+    <row r="23">
+      <c r="A23" s="2" t="n">
         <v>45261</v>
       </c>
-      <c r="B23">
+      <c r="B23" t="n">
         <v>46.2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="2">
+    <row r="24">
+      <c r="A24" s="2" t="n">
         <v>45292</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="n">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
+    <row r="25">
+      <c r="A25" s="2" t="n">
         <v>45323</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="n">
         <v>47.5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="2">
+    <row r="26">
+      <c r="A26" s="2" t="n">
         <v>45352</v>
       </c>
-      <c r="B26">
+      <c r="B26" t="n">
         <v>50.3</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="2">
+    <row r="27">
+      <c r="A27" s="2" t="n">
         <v>45383</v>
       </c>
-      <c r="B27">
+      <c r="B27" t="n">
         <v>49.1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="2">
+    <row r="28">
+      <c r="A28" s="2" t="n">
         <v>45413</v>
       </c>
-      <c r="B28">
+      <c r="B28" t="n">
         <v>51.2</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="2">
+    <row r="29">
+      <c r="A29" s="2" t="n">
         <v>45444</v>
       </c>
-      <c r="B29">
+      <c r="B29" t="n">
         <v>50.9</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="2">
+    <row r="30">
+      <c r="A30" s="2" t="n">
         <v>45474</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="n">
         <v>52.1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="2">
+    <row r="31">
+      <c r="A31" s="2" t="n">
         <v>45505</v>
       </c>
-      <c r="B31">
+      <c r="B31" t="n">
         <v>52.5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="2">
+    <row r="32">
+      <c r="A32" s="2" t="n">
         <v>45536</v>
       </c>
-      <c r="B32">
+      <c r="B32" t="n">
         <v>51.5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="2">
+    <row r="33">
+      <c r="A33" s="2" t="n">
         <v>45566</v>
       </c>
-      <c r="B33">
+      <c r="B33" t="n">
         <v>49.9</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="2">
+    <row r="34">
+      <c r="A34" s="2" t="n">
         <v>45597</v>
       </c>
-      <c r="B34">
+      <c r="B34" t="n">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="2">
+    <row r="35">
+      <c r="A35" s="2" t="n">
         <v>45627</v>
       </c>
-      <c r="B35">
+      <c r="B35" t="n">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="2">
+    <row r="36">
+      <c r="A36" s="2" t="n">
         <v>45658</v>
       </c>
-      <c r="B36">
+      <c r="B36" t="n">
         <v>48.3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="2">
+    <row r="37">
+      <c r="A37" s="2" t="n">
         <v>45689</v>
       </c>
-      <c r="B37">
+      <c r="B37" t="n">
         <v>46.9</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="2">
+    <row r="38">
+      <c r="A38" s="2" t="n">
         <v>45717</v>
       </c>
-      <c r="B38">
+      <c r="B38" t="n">
         <v>44.9</v>
       </c>
     </row>
@@ -788,127 +754,183 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B1" s="1">
+    <row r="1">
+      <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13">
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>points</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>original_source</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>S&amp;P Global</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>United Kingdom Manufacturing PMI</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>indicator</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>manufacturing pmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>country</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>united kingdom</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Trading Economics</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>united-kingdom/manufacturing-pmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Markit/CIPS UK Manufacturing Purchasing Managers’ Index measures the performance of the manufacturing sector and is derived from a survey of 600 industrial companies. The Manufacturing Purchasing Managers Index is based on five individual indexes with the following weights: New Orders (30 percent), Output (25 percent), Employment (20 percent), Suppliers’ Delivery Times (15 percent) and Stock of Items Purchased (10 percent), with the Delivery Times index inverted so that it moves in a comparable direction. A reading above 50 indicates an expansion of the manufacturing sector compared to the previous month; below 50 represents a contraction; while 50 indicates no change. This is only a limited sample of PMI headline data displayed on the Customer’s service, under licence from S&amp;P Global. Full historic PMI headline data and all other PMI sub-index data and histories are available on subscription from S&amp;P Global. Contact economics@spglobal.com for more details.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>frequency</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>start_date</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2022-03-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>end_date</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2025-03-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>min_value</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14">
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>max_value</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
         <v>55.8</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15">
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>length</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
         <v>37</v>
       </c>
     </row>

</xml_diff>